<commit_message>
msz - page keyw. select, selected, notsel...
</commit_message>
<xml_diff>
--- a/Data/Dialogs/dlgProfil.xlsx
+++ b/Data/Dialogs/dlgProfil.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\PycharmProjects\OnTop\Data\Dialogs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8B696A3-0157-4755-837C-C6979DECE219}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C469076-D433-4B2A-ACEC-325A87145B19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="372" yWindow="1320" windowWidth="40440" windowHeight="15300" xr2:uid="{AE079285-A10A-4E50-89E0-1FC0BD4174C7}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
   <si>
     <t>Control</t>
   </si>
@@ -72,13 +72,19 @@
     <t>Auswahl Page Profil</t>
   </si>
   <si>
-    <t>xpath=//*/li[@class = 'nav-item']/a[text()=" Benachrichtigungen"]</t>
-  </si>
-  <si>
-    <t>xpath=//*/li[@class = 'nav-item']/a[text()=' Abwesenheiten')]</t>
-  </si>
-  <si>
-    <t>xpath=//*/li[@class = 'nav-item']/a[text()=' Profil')]</t>
+    <t>&lt;SELECTED&gt;</t>
+  </si>
+  <si>
+    <t>&lt;NOTSELECTED&gt;</t>
+  </si>
+  <si>
+    <t>xpath=//*/li[@class = 'nav-item']/a[text()=' Profil']</t>
+  </si>
+  <si>
+    <t>xpath=//*/li[@class = 'nav-item']/a[text()=' Abwesenheiten']</t>
+  </si>
+  <si>
+    <t>xpath=//*/li[@class = 'nav-item']/a[text()=' Benachrichtigungen']</t>
   </si>
 </sst>
 </file>
@@ -482,7 +488,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -524,10 +530,10 @@
         <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F2" t="s">
         <v>2</v>
@@ -540,6 +546,15 @@
       <c r="B3" t="s">
         <v>5</v>
       </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
       <c r="F3" t="s">
         <v>9</v>
       </c>
@@ -588,6 +603,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
msz - some checkbox keywords
</commit_message>
<xml_diff>
--- a/Data/Dialogs/dlgProfil.xlsx
+++ b/Data/Dialogs/dlgProfil.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\PycharmProjects\OnTop\Data\Dialogs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C469076-D433-4B2A-ACEC-325A87145B19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9E92E2D-D48F-40A6-819F-9AB3436A216C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="372" yWindow="1320" windowWidth="40440" windowHeight="15300" xr2:uid="{AE079285-A10A-4E50-89E0-1FC0BD4174C7}"/>
+    <workbookView xWindow="840" yWindow="1980" windowWidth="40440" windowHeight="15300" xr2:uid="{AE079285-A10A-4E50-89E0-1FC0BD4174C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -488,7 +488,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
msz - Profil_Abwesenheiten_Normalfall_Anlage ok
</commit_message>
<xml_diff>
--- a/Data/Dialogs/dlgProfil.xlsx
+++ b/Data/Dialogs/dlgProfil.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\PycharmProjects\OnTop\Data\Dialogs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BB98D67-4711-4184-9164-2004231484C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F7A67E6-CA21-4033-AE5A-832666A62FBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="852" yWindow="780" windowWidth="37308" windowHeight="15300" xr2:uid="{AE079285-A10A-4E50-89E0-1FC0BD4174C7}"/>
+    <workbookView xWindow="3564" yWindow="1056" windowWidth="38676" windowHeight="15300" xr2:uid="{AE079285-A10A-4E50-89E0-1FC0BD4174C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="36">
   <si>
     <t>Action</t>
   </si>
@@ -126,10 +126,13 @@
     <t>//android.view.View[@content-desc=" Benachrichtigungen"]/android.widget.TextView[@text="Benachrichtigungen"]</t>
   </si>
   <si>
-    <t>//android.view.View[@content-desc=" Abwesenheiten"]/android.widget.TextView[@text="Abwesenheiten"]</t>
-  </si>
-  <si>
     <t>//android.view.View[@content-desc=" Geld verdienen"]/android.widget.TextView[@text="Geld verdienen"]</t>
+  </si>
+  <si>
+    <t>//android.webkit.WebView/android.widget.ListView</t>
+  </si>
+  <si>
+    <t>//android.webkit.WebView/android.widget.ListView//android.view.View[@content-desc=" Abwesenheiten"]/android.widget.TextView[@text="Abwesenheiten"]</t>
   </si>
 </sst>
 </file>
@@ -560,10 +563,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82737E07-8287-4E6B-9130-6C87B574EFB8}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -571,7 +574,7 @@
     <col min="1" max="1" width="47" customWidth="1"/>
     <col min="2" max="2" width="12.21875" customWidth="1"/>
     <col min="3" max="3" width="83.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="92" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="110.5546875" customWidth="1"/>
     <col min="5" max="5" width="99.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="91.33203125" bestFit="1" customWidth="1"/>
   </cols>
@@ -608,13 +611,13 @@
         <v>31</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>32</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G2" t="s">
         <v>0</v>
@@ -787,6 +790,11 @@
       </c>
       <c r="G13" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E18" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>